<commit_message>
initial commit for the branch
</commit_message>
<xml_diff>
--- a/GenLoc.xlsx
+++ b/GenLoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacos\Desktop\pyRepos\terrainGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8E6F7D-F425-4420-B8E6-14D455F8292C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D54A07-24DF-49BF-AF6A-E4E98137E2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="360" windowWidth="14055" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Tomb</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Nomad camp</t>
+  </si>
+  <si>
+    <t>Ocean</t>
+  </si>
+  <si>
+    <t>Shipwreck</t>
+  </si>
+  <si>
+    <t>Sucken Temple</t>
   </si>
 </sst>
 </file>
@@ -561,10 +570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D0F117-40AB-46C0-B036-56B78DCF36F6}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +581,7 @@
     <col min="1" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -588,8 +597,11 @@
       <c r="E1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -605,8 +617,11 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -622,8 +637,11 @@
       <c r="E3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -640,7 +658,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -657,7 +675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -674,7 +692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -685,7 +703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -693,7 +711,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -701,12 +719,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Updating genloc for desert biomes
</commit_message>
<xml_diff>
--- a/GenLoc.xlsx
+++ b/GenLoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacos\Desktop\pyRepos\terrainGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D54A07-24DF-49BF-AF6A-E4E98137E2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A40757C-7481-40AC-ACF6-65BB3061173D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="360" windowWidth="14055" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="90" windowWidth="14055" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>Tomb</t>
   </si>
@@ -143,6 +143,24 @@
   </si>
   <si>
     <t>Sucken Temple</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>Badlands</t>
+  </si>
+  <si>
+    <t>Cave</t>
+  </si>
+  <si>
+    <t>Oasis</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Abandoned Mine</t>
   </si>
 </sst>
 </file>
@@ -570,10 +588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D0F117-40AB-46C0-B036-56B78DCF36F6}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +599,7 @@
     <col min="1" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -600,8 +618,14 @@
       <c r="F1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -620,8 +644,14 @@
       <c r="F2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -640,8 +670,14 @@
       <c r="F3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -657,8 +693,14 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -674,8 +716,14 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -691,8 +739,14 @@
       <c r="E6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -702,31 +756,55 @@
       <c r="E7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
staging changes for main
</commit_message>
<xml_diff>
--- a/GenLoc.xlsx
+++ b/GenLoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacos\Desktop\pyRepos\terrainGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D54A07-24DF-49BF-AF6A-E4E98137E2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD35F81-EF86-434F-A527-C24FA6E813A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="360" windowWidth="14055" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14055" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>Tomb</t>
   </si>
@@ -143,6 +143,24 @@
   </si>
   <si>
     <t>Sucken Temple</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>Oasis</t>
+  </si>
+  <si>
+    <t>Badlands</t>
+  </si>
+  <si>
+    <t>Cave</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Abandoned Mine</t>
   </si>
 </sst>
 </file>
@@ -178,7 +196,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -570,10 +590,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D0F117-40AB-46C0-B036-56B78DCF36F6}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,7 +601,7 @@
     <col min="1" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -600,8 +620,14 @@
       <c r="F1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -620,8 +646,14 @@
       <c r="F2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -640,8 +672,14 @@
       <c r="F3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -657,8 +695,14 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -674,8 +718,14 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -691,8 +741,14 @@
       <c r="E6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -702,31 +758,55 @@
       <c r="E7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finishing up merge from islands branch
</commit_message>
<xml_diff>
--- a/GenLoc.xlsx
+++ b/GenLoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacos\Desktop\pyRepos\terrainGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A40757C-7481-40AC-ACF6-65BB3061173D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1BA08D-2138-4DF8-8D2B-5BD13374BCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="90" windowWidth="14055" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="30" windowWidth="14055" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>Tomb</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Abandoned Mine</t>
+  </si>
+  <si>
+    <t>Beach</t>
   </si>
 </sst>
 </file>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D0F117-40AB-46C0-B036-56B78DCF36F6}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +602,7 @@
     <col min="1" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -624,8 +627,11 @@
       <c r="H1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -650,8 +656,11 @@
       <c r="H2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -677,7 +686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -700,7 +709,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -723,7 +732,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -746,7 +755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -763,7 +772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -777,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -791,7 +800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -799,7 +808,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Updated some locations and added continents climate
</commit_message>
<xml_diff>
--- a/GenLoc.xlsx
+++ b/GenLoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacos\Desktop\pyRepos\terrainGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1BA08D-2138-4DF8-8D2B-5BD13374BCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D049FB-A957-4331-AAD5-C5B6E63A2BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="14055" windowHeight="10890" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>Tomb</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Beach</t>
+  </si>
+  <si>
+    <t>Major City</t>
+  </si>
+  <si>
+    <t>Port Village/City</t>
   </si>
 </sst>
 </file>
@@ -594,12 +600,12 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="20.7109375" customWidth="1"/>
+    <col min="1" max="9" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -685,6 +691,9 @@
       <c r="H3" t="s">
         <v>0</v>
       </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -762,6 +771,9 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
@@ -803,6 +815,9 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
       </c>
       <c r="H10" t="s">
         <v>43</v>

</xml_diff>